<commit_message>
Aktivne učinkovine in mikrobiološke to header format
</commit_message>
<xml_diff>
--- a/unstructTest.xlsx
+++ b/unstructTest.xlsx
@@ -1,13 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -86,7 +85,7 @@
     <t>čisto, suho skladišče</t>
   </si>
   <si>
-    <t>26.05.2009</t>
+    <t>26.05.2008</t>
   </si>
   <si>
     <t>s pihanjem oblikovano belo steklo (steklo ustreza III hidrolitski skupini ISO 719/85)</t>

</xml_diff>